<commit_message>
remake some bags... BUT IT`S FEATURE!! I KNOW! i know.....
</commit_message>
<xml_diff>
--- a/WebApplication14/wwwroot/e3a51807-d359-4547-bfaa-140f55c9611b.xlsx
+++ b/WebApplication14/wwwroot/e3a51807-d359-4547-bfaa-140f55c9611b.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -41,16 +41,10 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>Sony Headphones</t>
+    <t>Sony</t>
   </si>
   <si>
     <t>Ukraine</t>
-  </si>
-  <si>
-    <t>razor rz04</t>
-  </si>
-  <si>
-    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -96,7 +90,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -153,58 +147,18 @@
         <v>10</v>
       </c>
       <c r="D3" s="0">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E3" s="0">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="F3" s="0">
-        <v>48</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="0">
-        <v>23</v>
-      </c>
-      <c r="E4" s="0">
-        <v>25</v>
-      </c>
       <c r="F4" s="0">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0">
-        <v>23</v>
-      </c>
-      <c r="E5" s="0">
-        <v>25</v>
-      </c>
-      <c r="F5" s="0">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="F6" s="0">
-        <v>1438</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>